<commit_message>
Update AHB RTT Test Cases (2).xlsx
</commit_message>
<xml_diff>
--- a/AHB RTT Test Cases (2).xlsx
+++ b/AHB RTT Test Cases (2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hariprasad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hariprasad\Desktop\m-test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABB7FD1-32BA-4295-8DE1-A57CF1A748DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F3EFB0-E569-4B63-B8E7-F3375246371C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="212">
   <si>
     <t>Test case id</t>
   </si>
@@ -660,6 +660,9 @@
   </si>
   <si>
     <t>I observed AHB Yellow RTT is should not Active</t>
+  </si>
+  <si>
+    <t>df</t>
   </si>
 </sst>
 </file>
@@ -3149,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3228,6 +3231,12 @@
       <c r="A4" s="7">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
       <c r="G4" s="4" t="s">
         <v>127</v>
       </c>

</xml_diff>